<commit_message>
chore: string to float
</commit_message>
<xml_diff>
--- a/Plantillas modelos impuestos UHY.xlsx
+++ b/Plantillas modelos impuestos UHY.xlsx
@@ -1897,10 +1897,8 @@
       <c r="H8" s="26" t="n"/>
       <c r="I8" s="26" t="n"/>
       <c r="J8" s="30" t="n"/>
-      <c r="K8" s="27" t="inlineStr">
-        <is>
-          <t>539,49</t>
-        </is>
+      <c r="K8" s="27" t="n">
+        <v>539.49</v>
       </c>
       <c r="L8" s="27" t="n"/>
       <c r="M8" s="27" t="n"/>
@@ -1935,10 +1933,8 @@
       <c r="H9" s="27" t="n"/>
       <c r="I9" s="27" t="n"/>
       <c r="J9" s="27" t="n"/>
-      <c r="K9" s="27" t="inlineStr">
-        <is>
-          <t>878.121,61</t>
-        </is>
+      <c r="K9" s="27" t="n">
+        <v>878121.61</v>
       </c>
       <c r="L9" s="27" t="n"/>
       <c r="M9" s="27" t="n"/>
@@ -1973,10 +1969,8 @@
       <c r="H10" s="27" t="n"/>
       <c r="I10" s="27" t="n"/>
       <c r="J10" s="27" t="n"/>
-      <c r="K10" s="27" t="inlineStr">
-        <is>
-          <t>1.523,96</t>
-        </is>
+      <c r="K10" s="27" t="n">
+        <v>1523.96</v>
       </c>
       <c r="L10" s="27" t="n"/>
       <c r="M10" s="27" t="n"/>
@@ -2045,10 +2039,8 @@
       <c r="H12" s="33" t="n"/>
       <c r="I12" s="33" t="n"/>
       <c r="J12" s="33" t="n"/>
-      <c r="K12" s="33" t="inlineStr">
-        <is>
-          <t>-44.504,79</t>
-        </is>
+      <c r="K12" s="33" t="n">
+        <v>-44504.79</v>
       </c>
       <c r="L12" s="33" t="n"/>
       <c r="M12" s="33" t="n"/>
@@ -2320,10 +2312,8 @@
       <c r="H20" s="27" t="n"/>
       <c r="I20" s="27" t="n"/>
       <c r="J20" s="27" t="n"/>
-      <c r="K20" s="27" t="inlineStr">
-        <is>
-          <t>53,96</t>
-        </is>
+      <c r="K20" s="27" t="n">
+        <v>53.96</v>
       </c>
       <c r="L20" s="27" t="n"/>
       <c r="M20" s="27" t="n"/>
@@ -2358,10 +2348,8 @@
       <c r="H21" s="27" t="n"/>
       <c r="I21" s="27" t="n"/>
       <c r="J21" s="27" t="n"/>
-      <c r="K21" s="27" t="inlineStr">
-        <is>
-          <t>184.406,17</t>
-        </is>
+      <c r="K21" s="27" t="n">
+        <v>184406.17</v>
       </c>
       <c r="L21" s="27" t="n"/>
       <c r="M21" s="27" t="n"/>
@@ -2396,10 +2384,8 @@
       <c r="H22" s="27" t="n"/>
       <c r="I22" s="27" t="n"/>
       <c r="J22" s="27" t="n"/>
-      <c r="K22" s="27" t="inlineStr">
-        <is>
-          <t>320,03</t>
-        </is>
+      <c r="K22" s="27" t="n">
+        <v>320.03</v>
       </c>
       <c r="L22" s="27" t="n"/>
       <c r="M22" s="27" t="n"/>
@@ -2468,10 +2454,8 @@
       <c r="H24" s="33" t="n"/>
       <c r="I24" s="33" t="n"/>
       <c r="J24" s="33" t="n"/>
-      <c r="K24" s="33" t="inlineStr">
-        <is>
-          <t>-9.344,28</t>
-        </is>
+      <c r="K24" s="33" t="n">
+        <v>-9344.280000000001</v>
       </c>
       <c r="L24" s="33" t="n"/>
       <c r="M24" s="33" t="n"/>
@@ -2709,10 +2693,8 @@
       <c r="H31" s="27" t="n"/>
       <c r="I31" s="27" t="n"/>
       <c r="J31" s="27" t="n"/>
-      <c r="K31" s="27" t="inlineStr">
-        <is>
-          <t>789.653,47</t>
-        </is>
+      <c r="K31" s="27" t="n">
+        <v>789653.47</v>
       </c>
       <c r="L31" s="27" t="n"/>
       <c r="M31" s="27" t="n"/>
@@ -2747,10 +2729,8 @@
       <c r="H32" s="27" t="n"/>
       <c r="I32" s="27" t="n"/>
       <c r="J32" s="27" t="n"/>
-      <c r="K32" s="27" t="inlineStr">
-        <is>
-          <t>978,00</t>
-        </is>
+      <c r="K32" s="27" t="n">
+        <v>978</v>
       </c>
       <c r="L32" s="27" t="n"/>
       <c r="M32" s="27" t="n"/>
@@ -2853,10 +2833,8 @@
       <c r="H35" s="27" t="n"/>
       <c r="I35" s="27" t="n"/>
       <c r="J35" s="27" t="n"/>
-      <c r="K35" s="27" t="inlineStr">
-        <is>
-          <t>1.523,96</t>
-        </is>
+      <c r="K35" s="27" t="n">
+        <v>1523.96</v>
       </c>
       <c r="L35" s="27" t="n"/>
       <c r="M35" s="27" t="n"/>
@@ -2925,10 +2903,8 @@
       <c r="H37" s="27" t="n"/>
       <c r="I37" s="27" t="n"/>
       <c r="J37" s="27" t="n"/>
-      <c r="K37" s="27" t="inlineStr">
-        <is>
-          <t>-127.211,56</t>
-        </is>
+      <c r="K37" s="27" t="n">
+        <v>-127211.56</v>
       </c>
       <c r="L37" s="27" t="n"/>
       <c r="M37" s="27" t="n"/>
@@ -3059,10 +3035,8 @@
       <c r="H41" s="27" t="n"/>
       <c r="I41" s="27" t="n"/>
       <c r="J41" s="27" t="n"/>
-      <c r="K41" s="27" t="inlineStr">
-        <is>
-          <t>165.739,60</t>
-        </is>
+      <c r="K41" s="27" t="n">
+        <v>165739.6</v>
       </c>
       <c r="L41" s="27" t="n"/>
       <c r="M41" s="27" t="n"/>
@@ -3097,10 +3071,8 @@
       <c r="H42" s="27" t="n"/>
       <c r="I42" s="27" t="n"/>
       <c r="J42" s="27" t="n"/>
-      <c r="K42" s="27" t="inlineStr">
-        <is>
-          <t>205,38</t>
-        </is>
+      <c r="K42" s="27" t="n">
+        <v>205.38</v>
       </c>
       <c r="L42" s="27" t="n"/>
       <c r="M42" s="27" t="n"/>
@@ -3203,10 +3175,8 @@
       <c r="H45" s="27" t="n"/>
       <c r="I45" s="27" t="n"/>
       <c r="J45" s="27" t="n"/>
-      <c r="K45" s="27" t="inlineStr">
-        <is>
-          <t>320,03</t>
-        </is>
+      <c r="K45" s="27" t="n">
+        <v>320.03</v>
       </c>
       <c r="L45" s="27" t="n"/>
       <c r="M45" s="27" t="n"/>
@@ -3275,10 +3245,8 @@
       <c r="H47" s="27" t="n"/>
       <c r="I47" s="27" t="n"/>
       <c r="J47" s="27" t="n"/>
-      <c r="K47" s="27" t="inlineStr">
-        <is>
-          <t>-26.714,41</t>
-        </is>
+      <c r="K47" s="27" t="n">
+        <v>-26714.41</v>
       </c>
       <c r="L47" s="27" t="n"/>
       <c r="M47" s="27" t="n"/>

</xml_diff>

<commit_message>
chore: fixed upload pdf
</commit_message>
<xml_diff>
--- a/Plantillas modelos impuestos UHY.xlsx
+++ b/Plantillas modelos impuestos UHY.xlsx
@@ -3692,10 +3692,8 @@
       <c r="H61" s="27" t="n"/>
       <c r="I61" s="27" t="n"/>
       <c r="J61" s="27" t="n"/>
-      <c r="K61" s="27" t="inlineStr">
-        <is>
-          <t>1.949,52</t>
-        </is>
+      <c r="K61" s="27" t="n">
+        <v>1949.52</v>
       </c>
       <c r="L61" s="27" t="n"/>
       <c r="M61" s="27" t="n"/>
@@ -3730,10 +3728,8 @@
       <c r="H62" s="27" t="n"/>
       <c r="I62" s="27" t="n"/>
       <c r="J62" s="27" t="n"/>
-      <c r="K62" s="27" t="inlineStr">
-        <is>
-          <t>12.432,50</t>
-        </is>
+      <c r="K62" s="27" t="n">
+        <v>12432.5</v>
       </c>
       <c r="L62" s="27" t="n"/>
       <c r="M62" s="27" t="n"/>

</xml_diff>

<commit_message>
chore: working upload multiplefiles
</commit_message>
<xml_diff>
--- a/Plantillas modelos impuestos UHY.xlsx
+++ b/Plantillas modelos impuestos UHY.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="notas " sheetId="1" state="visible" r:id="rId1"/>
@@ -1679,7 +1679,7 @@
       <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="3.77734375" customWidth="1" style="70" min="1" max="1"/>
     <col width="18.77734375" customWidth="1" style="70" min="2" max="2"/>
@@ -1900,8 +1900,12 @@
       <c r="K8" s="27" t="n">
         <v>539.49</v>
       </c>
-      <c r="L8" s="27" t="n"/>
-      <c r="M8" s="27" t="n"/>
+      <c r="L8" s="27" t="n">
+        <v>539.49</v>
+      </c>
+      <c r="M8" s="27" t="n">
+        <v>539.49</v>
+      </c>
       <c r="N8" s="27" t="n"/>
       <c r="O8" s="27" t="n"/>
       <c r="P8" s="27" t="n"/>
@@ -1936,8 +1940,12 @@
       <c r="K9" s="27" t="n">
         <v>878121.61</v>
       </c>
-      <c r="L9" s="27" t="n"/>
-      <c r="M9" s="27" t="n"/>
+      <c r="L9" s="27" t="n">
+        <v>878121.61</v>
+      </c>
+      <c r="M9" s="27" t="n">
+        <v>878121.61</v>
+      </c>
       <c r="N9" s="27" t="n"/>
       <c r="O9" s="27" t="n"/>
       <c r="P9" s="26" t="n"/>
@@ -1972,8 +1980,12 @@
       <c r="K10" s="27" t="n">
         <v>1523.96</v>
       </c>
-      <c r="L10" s="27" t="n"/>
-      <c r="M10" s="27" t="n"/>
+      <c r="L10" s="27" t="n">
+        <v>1523.96</v>
+      </c>
+      <c r="M10" s="27" t="n">
+        <v>1523.96</v>
+      </c>
       <c r="N10" s="27" t="n"/>
       <c r="O10" s="27" t="n"/>
       <c r="P10" s="27" t="n"/>
@@ -2042,8 +2054,12 @@
       <c r="K12" s="33" t="n">
         <v>-44504.79</v>
       </c>
-      <c r="L12" s="33" t="n"/>
-      <c r="M12" s="33" t="n"/>
+      <c r="L12" s="33" t="n">
+        <v>-44504.79</v>
+      </c>
+      <c r="M12" s="33" t="n">
+        <v>-44504.79</v>
+      </c>
       <c r="N12" s="33" t="n"/>
       <c r="O12" s="33" t="n"/>
       <c r="P12" s="33" t="n"/>
@@ -2315,8 +2331,12 @@
       <c r="K20" s="27" t="n">
         <v>53.96</v>
       </c>
-      <c r="L20" s="27" t="n"/>
-      <c r="M20" s="27" t="n"/>
+      <c r="L20" s="27" t="n">
+        <v>53.96</v>
+      </c>
+      <c r="M20" s="27" t="n">
+        <v>53.96</v>
+      </c>
       <c r="N20" s="27" t="n"/>
       <c r="O20" s="27" t="n"/>
       <c r="P20" s="27" t="n"/>
@@ -2351,8 +2371,12 @@
       <c r="K21" s="27" t="n">
         <v>184406.17</v>
       </c>
-      <c r="L21" s="27" t="n"/>
-      <c r="M21" s="27" t="n"/>
+      <c r="L21" s="27" t="n">
+        <v>184406.17</v>
+      </c>
+      <c r="M21" s="27" t="n">
+        <v>184406.17</v>
+      </c>
       <c r="N21" s="27" t="n"/>
       <c r="O21" s="27" t="n"/>
       <c r="P21" s="27" t="n"/>
@@ -2387,8 +2411,12 @@
       <c r="K22" s="27" t="n">
         <v>320.03</v>
       </c>
-      <c r="L22" s="27" t="n"/>
-      <c r="M22" s="27" t="n"/>
+      <c r="L22" s="27" t="n">
+        <v>320.03</v>
+      </c>
+      <c r="M22" s="27" t="n">
+        <v>320.03</v>
+      </c>
       <c r="N22" s="27" t="n"/>
       <c r="O22" s="27" t="n"/>
       <c r="P22" s="27" t="n"/>
@@ -2457,8 +2485,12 @@
       <c r="K24" s="33" t="n">
         <v>-9344.280000000001</v>
       </c>
-      <c r="L24" s="33" t="n"/>
-      <c r="M24" s="33" t="n"/>
+      <c r="L24" s="33" t="n">
+        <v>-9344.280000000001</v>
+      </c>
+      <c r="M24" s="33" t="n">
+        <v>-9344.280000000001</v>
+      </c>
       <c r="N24" s="33" t="n"/>
       <c r="O24" s="33" t="n"/>
       <c r="P24" s="33" t="n"/>
@@ -2696,8 +2728,12 @@
       <c r="K31" s="27" t="n">
         <v>789653.47</v>
       </c>
-      <c r="L31" s="27" t="n"/>
-      <c r="M31" s="27" t="n"/>
+      <c r="L31" s="27" t="n">
+        <v>789653.47</v>
+      </c>
+      <c r="M31" s="27" t="n">
+        <v>789653.47</v>
+      </c>
       <c r="N31" s="27" t="n"/>
       <c r="O31" s="27" t="n"/>
       <c r="P31" s="27" t="n"/>
@@ -2732,8 +2768,12 @@
       <c r="K32" s="27" t="n">
         <v>978</v>
       </c>
-      <c r="L32" s="27" t="n"/>
-      <c r="M32" s="27" t="n"/>
+      <c r="L32" s="27" t="n">
+        <v>978</v>
+      </c>
+      <c r="M32" s="27" t="n">
+        <v>978</v>
+      </c>
       <c r="N32" s="27" t="n"/>
       <c r="O32" s="27" t="n"/>
       <c r="P32" s="27" t="n"/>
@@ -2836,8 +2876,12 @@
       <c r="K35" s="27" t="n">
         <v>1523.96</v>
       </c>
-      <c r="L35" s="27" t="n"/>
-      <c r="M35" s="27" t="n"/>
+      <c r="L35" s="27" t="n">
+        <v>1523.96</v>
+      </c>
+      <c r="M35" s="27" t="n">
+        <v>1523.96</v>
+      </c>
       <c r="N35" s="27" t="n"/>
       <c r="O35" s="27" t="n"/>
       <c r="P35" s="27" t="n"/>
@@ -2906,8 +2950,12 @@
       <c r="K37" s="27" t="n">
         <v>-127211.56</v>
       </c>
-      <c r="L37" s="27" t="n"/>
-      <c r="M37" s="27" t="n"/>
+      <c r="L37" s="27" t="n">
+        <v>-127211.56</v>
+      </c>
+      <c r="M37" s="27" t="n">
+        <v>-127211.56</v>
+      </c>
       <c r="N37" s="27" t="n"/>
       <c r="O37" s="27" t="n"/>
       <c r="P37" s="27" t="n"/>
@@ -3038,8 +3086,12 @@
       <c r="K41" s="27" t="n">
         <v>165739.6</v>
       </c>
-      <c r="L41" s="27" t="n"/>
-      <c r="M41" s="27" t="n"/>
+      <c r="L41" s="27" t="n">
+        <v>165739.6</v>
+      </c>
+      <c r="M41" s="27" t="n">
+        <v>165739.6</v>
+      </c>
       <c r="N41" s="27" t="n"/>
       <c r="O41" s="27" t="n"/>
       <c r="P41" s="27" t="n"/>
@@ -3074,8 +3126,12 @@
       <c r="K42" s="27" t="n">
         <v>205.38</v>
       </c>
-      <c r="L42" s="27" t="n"/>
-      <c r="M42" s="27" t="n"/>
+      <c r="L42" s="27" t="n">
+        <v>205.38</v>
+      </c>
+      <c r="M42" s="27" t="n">
+        <v>205.38</v>
+      </c>
       <c r="N42" s="27" t="n"/>
       <c r="O42" s="27" t="n"/>
       <c r="P42" s="27" t="n"/>
@@ -3178,8 +3234,12 @@
       <c r="K45" s="27" t="n">
         <v>320.03</v>
       </c>
-      <c r="L45" s="27" t="n"/>
-      <c r="M45" s="27" t="n"/>
+      <c r="L45" s="27" t="n">
+        <v>320.03</v>
+      </c>
+      <c r="M45" s="27" t="n">
+        <v>320.03</v>
+      </c>
       <c r="N45" s="27" t="n"/>
       <c r="O45" s="27" t="n"/>
       <c r="P45" s="27" t="n"/>
@@ -3248,8 +3308,12 @@
       <c r="K47" s="27" t="n">
         <v>-26714.41</v>
       </c>
-      <c r="L47" s="27" t="n"/>
-      <c r="M47" s="27" t="n"/>
+      <c r="L47" s="27" t="n">
+        <v>-26714.41</v>
+      </c>
+      <c r="M47" s="27" t="n">
+        <v>-26714.41</v>
+      </c>
       <c r="N47" s="27" t="n"/>
       <c r="O47" s="27" t="n"/>
       <c r="P47" s="27" t="n"/>
@@ -3567,8 +3631,16 @@
           <t>35.885,28</t>
         </is>
       </c>
-      <c r="L57" s="27" t="n"/>
-      <c r="M57" s="27" t="n"/>
+      <c r="L57" s="27" t="inlineStr">
+        <is>
+          <t>35.885,28</t>
+        </is>
+      </c>
+      <c r="M57" s="27" t="inlineStr">
+        <is>
+          <t>35.885,28</t>
+        </is>
+      </c>
       <c r="N57" s="27" t="n"/>
       <c r="O57" s="27" t="n"/>
       <c r="P57" s="27" t="n"/>
@@ -3695,8 +3767,12 @@
       <c r="K61" s="27" t="n">
         <v>1949.52</v>
       </c>
-      <c r="L61" s="27" t="n"/>
-      <c r="M61" s="27" t="n"/>
+      <c r="L61" s="27" t="n">
+        <v>1949.52</v>
+      </c>
+      <c r="M61" s="27" t="n">
+        <v>1949.52</v>
+      </c>
       <c r="N61" s="27" t="n"/>
       <c r="O61" s="27" t="n"/>
       <c r="P61" s="27" t="n"/>
@@ -3731,8 +3807,12 @@
       <c r="K62" s="27" t="n">
         <v>12432.5</v>
       </c>
-      <c r="L62" s="27" t="n"/>
-      <c r="M62" s="27" t="n"/>
+      <c r="L62" s="27" t="n">
+        <v>12432.5</v>
+      </c>
+      <c r="M62" s="27" t="n">
+        <v>12432.5</v>
+      </c>
       <c r="N62" s="27" t="n"/>
       <c r="O62" s="27" t="n"/>
       <c r="P62" s="27" t="n"/>
@@ -4484,7 +4564,7 @@
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="3.77734375" customWidth="1" style="70" min="1" max="1"/>
     <col width="49.21875" customWidth="1" style="70" min="2" max="2"/>
@@ -4666,7 +4746,9 @@
       <c r="G8" s="135" t="n"/>
       <c r="H8" s="135" t="n"/>
       <c r="I8" s="135" t="n"/>
-      <c r="J8" s="135" t="n"/>
+      <c r="J8" s="135" t="n">
+        <v>50</v>
+      </c>
       <c r="K8" s="135" t="n"/>
       <c r="L8" s="135" t="n"/>
       <c r="M8" s="135" t="n"/>
@@ -4700,7 +4782,9 @@
       <c r="G9" s="27" t="n"/>
       <c r="H9" s="27" t="n"/>
       <c r="I9" s="27" t="n"/>
-      <c r="J9" s="27" t="n"/>
+      <c r="J9" s="27" t="n">
+        <v>91023.50999999999</v>
+      </c>
       <c r="K9" s="27" t="n"/>
       <c r="L9" s="27" t="n"/>
       <c r="M9" s="27" t="n"/>
@@ -4733,7 +4817,9 @@
       <c r="G10" s="52" t="n"/>
       <c r="H10" s="52" t="n"/>
       <c r="I10" s="52" t="n"/>
-      <c r="J10" s="52" t="n"/>
+      <c r="J10" s="52" t="n">
+        <v>2825.92</v>
+      </c>
       <c r="K10" s="52" t="n"/>
       <c r="L10" s="52" t="n"/>
       <c r="M10" s="52" t="n"/>
@@ -5023,7 +5109,9 @@
       <c r="G20" s="135" t="n"/>
       <c r="H20" s="135" t="n"/>
       <c r="I20" s="135" t="n"/>
-      <c r="J20" s="135" t="n"/>
+      <c r="J20" s="135" t="n">
+        <v>4</v>
+      </c>
       <c r="K20" s="135" t="n"/>
       <c r="L20" s="135" t="n"/>
       <c r="M20" s="135" t="n"/>
@@ -5053,7 +5141,9 @@
       <c r="G21" s="27" t="n"/>
       <c r="H21" s="27" t="n"/>
       <c r="I21" s="27" t="n"/>
-      <c r="J21" s="27" t="n"/>
+      <c r="J21" s="27" t="n">
+        <v>1629.85</v>
+      </c>
       <c r="K21" s="27" t="n"/>
       <c r="L21" s="27" t="n"/>
       <c r="M21" s="27" t="n"/>
@@ -5083,7 +5173,9 @@
       <c r="G22" s="52" t="n"/>
       <c r="H22" s="52" t="n"/>
       <c r="I22" s="52" t="n"/>
-      <c r="J22" s="52" t="n"/>
+      <c r="J22" s="52" t="n">
+        <v>128.3</v>
+      </c>
       <c r="K22" s="52" t="n"/>
       <c r="L22" s="52" t="n"/>
       <c r="M22" s="52" t="n"/>
@@ -6843,7 +6935,7 @@
       <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="3.77734375" customWidth="1" style="70" min="1" max="1"/>
     <col width="36.5546875" customWidth="1" style="70" min="2" max="2"/>
@@ -7479,7 +7571,7 @@
       <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="12.5546875" customWidth="1" style="181" min="1" max="1"/>
     <col width="24" customWidth="1" style="181" min="2" max="2"/>
@@ -11828,7 +11920,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="3.77734375" customWidth="1" style="190" min="1" max="1"/>
     <col width="22.33203125" customWidth="1" style="190" min="2" max="2"/>
@@ -12373,7 +12465,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="12.6640625" customWidth="1" style="190" min="1" max="16384"/>
   </cols>
@@ -13138,7 +13230,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="12.6640625" customWidth="1" style="223" min="1" max="1"/>
     <col width="16" customWidth="1" style="223" min="2" max="2"/>

</xml_diff>